<commit_message>
all updated with check data; figs 1, 3, 4, 5,6,7 7alt,8,9,10 are done
</commit_message>
<xml_diff>
--- a/data/Meta-Analysis Data Collection.xlsx
+++ b/data/Meta-Analysis Data Collection.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\My Documents\Research\paul_genever_lab\alison_w\jan_2020\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emma Rand\Desktop\research\alison_w\alison_stemcell_reg\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5FF23FB-B7E8-48BD-830B-23CDA0E6A2A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="16665" windowHeight="6945"/>
+    <workbookView xWindow="12" yWindow="0" windowWidth="23016" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -25,6 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Ref #'!$A$1:$A$88</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -3625,7 +3627,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4489,6 +4491,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4524,6 +4543,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4699,101 +4735,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CE86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="AV1" sqref="AV1"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="102" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" style="102" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="102" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" style="102" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" style="102" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="102" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="102" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="102" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" style="102" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="102" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="102" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="102" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" style="102" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" style="102" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="102" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.44140625" style="102" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" style="102" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" style="102" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" style="102" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.88671875" style="102" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" style="103" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" style="102" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" style="102" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.5703125" style="102" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" style="102" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" style="102" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.5546875" style="102" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" style="102" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="8.7109375" style="102" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.28515625" style="102" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.140625" style="102" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.42578125" style="102" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.7109375" style="102" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="8.6640625" style="102" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.33203125" style="102" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.109375" style="102" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.44140625" style="102" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" style="102" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11" style="102" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.140625" style="102" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.85546875" style="104" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.28515625" style="104" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.85546875" style="104" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.85546875" style="102" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.28515625" style="102" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.85546875" style="102" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.85546875" style="104" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.140625" style="104" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.5703125" style="104" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.109375" style="102" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.88671875" style="104" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.33203125" style="104" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.88671875" style="104" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.88671875" style="102" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.33203125" style="102" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.88671875" style="102" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.88671875" style="104" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.109375" style="104" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.5546875" style="104" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="11" style="102" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.28515625" style="102" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.85546875" style="102" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.33203125" style="102" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.88671875" style="102" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="11" style="104" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.28515625" style="104" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.85546875" style="104" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.85546875" style="102" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.140625" style="102" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10.7109375" style="102" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.33203125" style="104" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.88671875" style="104" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.88671875" style="102" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.109375" style="102" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.6640625" style="102" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="11" style="104" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.28515625" style="104" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.85546875" style="104" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.85546875" style="102" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="10.140625" style="105" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.7109375" style="102" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.33203125" style="104" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.88671875" style="104" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.88671875" style="102" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="10.109375" style="105" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.6640625" style="102" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="11" style="104" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.28515625" style="106" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="9.85546875" style="104" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="12.85546875" style="102" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="11.140625" style="105" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="11.7109375" style="102" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="10.28515625" style="99" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="11.28515625" style="99" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="9.28515625" style="105" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="11.85546875" style="104" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.140625" style="104" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="10.7109375" style="104" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="11.85546875" style="102" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.140625" style="102" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="10.7109375" style="102" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.33203125" style="106" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="9.88671875" style="104" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="12.88671875" style="102" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="11.109375" style="105" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.6640625" style="102" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="10.33203125" style="99" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="11.33203125" style="99" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="9.33203125" style="105" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="11.88671875" style="104" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.109375" style="104" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="10.6640625" style="104" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="11.88671875" style="102" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.109375" style="102" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="10.6640625" style="102" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="11" style="102" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="11.28515625" style="107" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="11.7109375" style="107" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="14.140625" style="108" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="9.28515625" style="106" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="9.85546875" style="106" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="10.140625" style="106" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="10.140625" style="105" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="12.28515625" style="99" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="13.28515625" style="100" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="11.28515625" style="106" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="11.33203125" style="107" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="11.6640625" style="107" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="14.109375" style="108" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="9.33203125" style="106" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="9.88671875" style="106" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="10.109375" style="106" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="10.109375" style="105" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="12.33203125" style="99" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="13.33203125" style="100" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="11.33203125" style="106" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="11" style="105" bestFit="1" customWidth="1"/>
-    <col min="76" max="78" width="2.7109375" style="102" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="12.28515625" style="102" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="32.7109375" style="109" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="17.42578125" style="109" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="199.7109375" style="101" bestFit="1" customWidth="1"/>
-    <col min="84" max="16384" width="8.85546875" style="102"/>
+    <col min="76" max="78" width="2.6640625" style="102" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="12.33203125" style="102" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="32.6640625" style="109" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="17.44140625" style="109" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="199.6640625" style="101" bestFit="1" customWidth="1"/>
+    <col min="84" max="16384" width="8.88671875" style="102"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" s="140" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:83" s="140" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="138" t="s">
         <v>8</v>
       </c>
@@ -5044,7 +5080,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:83" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:83" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="102">
         <v>1</v>
       </c>
@@ -5244,7 +5280,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="3" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="102">
         <v>2</v>
       </c>
@@ -5453,7 +5489,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="4" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:83" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="102">
         <v>3</v>
       </c>
@@ -5656,7 +5692,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="5" spans="1:83" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:83" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="102">
         <v>4</v>
       </c>
@@ -5796,7 +5832,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:83" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A6" s="102">
         <v>5</v>
       </c>
@@ -5978,7 +6014,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A7" s="102">
         <v>6</v>
       </c>
@@ -6139,7 +6175,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A8" s="102">
         <v>7</v>
       </c>
@@ -6273,7 +6309,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:83" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A9" s="102">
         <v>8</v>
       </c>
@@ -6452,7 +6488,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="10" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A10" s="102">
         <v>9</v>
       </c>
@@ -6601,7 +6637,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:83" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A11" s="102">
         <v>10</v>
       </c>
@@ -6783,7 +6819,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="12" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="114">
         <v>11</v>
       </c>
@@ -6896,7 +6932,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="13" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A13" s="102">
         <v>12</v>
       </c>
@@ -7064,7 +7100,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="14" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A14" s="102">
         <v>13</v>
       </c>
@@ -7249,7 +7285,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="15" spans="1:83" s="114" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:83" s="114" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="114">
         <v>14</v>
       </c>
@@ -7401,7 +7437,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="16" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A16" s="102">
         <v>15</v>
       </c>
@@ -7556,7 +7592,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A17" s="102">
         <v>16</v>
       </c>
@@ -7656,7 +7692,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="18" spans="1:83" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A18" s="102">
         <v>17</v>
       </c>
@@ -7856,7 +7892,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="19" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A19" s="102">
         <v>18</v>
       </c>
@@ -7992,7 +8028,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="20" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A20" s="102">
         <v>19</v>
       </c>
@@ -8141,7 +8177,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A21" s="102">
         <v>20</v>
       </c>
@@ -8287,7 +8323,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A22" s="102">
         <v>21</v>
       </c>
@@ -8451,7 +8487,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A23" s="102">
         <v>22</v>
       </c>
@@ -8588,7 +8624,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A24" s="102">
         <v>23</v>
       </c>
@@ -8734,7 +8770,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="25" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A25" s="102">
         <v>24</v>
       </c>
@@ -8877,7 +8913,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:83" s="105" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:83" s="105" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" s="105">
         <v>25</v>
       </c>
@@ -9072,7 +9108,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="27" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A27" s="102">
         <v>26</v>
       </c>
@@ -9212,7 +9248,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A28" s="102">
         <v>27</v>
       </c>
@@ -9367,7 +9403,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:83" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A29" s="102">
         <v>28</v>
       </c>
@@ -9516,7 +9552,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="30" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A30" s="102">
         <v>29</v>
       </c>
@@ -9674,7 +9710,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="31" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A31" s="102">
         <v>30</v>
       </c>
@@ -9844,7 +9880,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A32" s="102">
         <v>31</v>
       </c>
@@ -9993,7 +10029,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="33" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A33" s="102">
         <v>32</v>
       </c>
@@ -10156,7 +10192,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A34" s="102">
         <v>33</v>
       </c>
@@ -10296,7 +10332,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A35" s="102">
         <v>34</v>
       </c>
@@ -10436,7 +10472,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="36" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A36" s="102">
         <v>35</v>
       </c>
@@ -10582,7 +10618,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="37" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A37" s="102">
         <v>36</v>
       </c>
@@ -10731,7 +10767,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="38" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A38" s="102">
         <v>37</v>
       </c>
@@ -10922,7 +10958,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="39" spans="1:83" s="120" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:83" s="120" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="120">
         <v>38</v>
       </c>
@@ -11051,7 +11087,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="40" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A40" s="102">
         <v>39</v>
       </c>
@@ -11209,7 +11245,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:83" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:83" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" s="102">
         <v>40</v>
       </c>
@@ -11403,7 +11439,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="42" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A42" s="102">
         <v>41</v>
       </c>
@@ -11546,7 +11582,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="43" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A43" s="102">
         <v>42</v>
       </c>
@@ -11698,7 +11734,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A44" s="102">
         <v>43</v>
       </c>
@@ -11893,7 +11929,7 @@
       </c>
       <c r="CE44" s="107"/>
     </row>
-    <row r="45" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A45" s="102">
         <v>44</v>
       </c>
@@ -12111,7 +12147,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="46" spans="1:83" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:83" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="102">
         <v>45</v>
       </c>
@@ -12266,7 +12302,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="47" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="114">
         <v>46</v>
       </c>
@@ -12463,7 +12499,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="48" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="114">
         <v>47</v>
       </c>
@@ -12675,7 +12711,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="114">
         <v>48</v>
       </c>
@@ -12836,7 +12872,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="114">
         <v>49</v>
       </c>
@@ -12985,7 +13021,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="51" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:83" x14ac:dyDescent="0.3">
       <c r="A51" s="102">
         <v>50</v>
       </c>
@@ -13134,7 +13170,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="52" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="114">
         <v>51</v>
       </c>
@@ -13295,7 +13331,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:83" s="105" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:83" s="105" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="105">
         <v>52</v>
       </c>
@@ -13487,7 +13523,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="54" spans="1:83" s="105" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:83" s="105" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="105">
         <v>53</v>
       </c>
@@ -13636,7 +13672,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="55" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="114">
         <v>54</v>
       </c>
@@ -13782,7 +13818,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="114">
         <v>55</v>
       </c>
@@ -13931,7 +13967,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="57" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="114">
         <v>56</v>
       </c>
@@ -14086,7 +14122,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="58" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:83" s="114" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="114">
         <v>57</v>
       </c>
@@ -14235,7 +14271,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="59" spans="1:83" s="98" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:83" s="98" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="98">
         <v>58</v>
       </c>
@@ -14417,7 +14453,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="60" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -14575,7 +14611,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="61" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -14757,7 +14793,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -14903,7 +14939,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -15058,7 +15094,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="64" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -15252,7 +15288,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="65" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -15329,7 +15365,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="66" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -15478,7 +15514,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="67" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -15633,7 +15669,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="68" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -15788,7 +15824,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="69" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -15940,7 +15976,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="70" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -16089,7 +16125,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="71" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -16244,7 +16280,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="72" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -16420,7 +16456,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -16566,7 +16602,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -16712,7 +16748,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -16915,7 +16951,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="76" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -17094,7 +17130,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="77" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -17294,7 +17330,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="78" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -17494,7 +17530,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="79" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -17682,7 +17718,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -17855,7 +17891,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="81" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -18004,7 +18040,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="82" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -18150,7 +18186,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="83" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -18296,7 +18332,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="84" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -18454,7 +18490,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="85" spans="1:83" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:83" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -18531,81 +18567,81 @@
         <v>827</v>
       </c>
     </row>
-    <row r="86" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:83" x14ac:dyDescent="0.3">
       <c r="T86"/>
     </row>
   </sheetData>
   <dataValidations count="24">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BY21:CA22 BY2:BZ20 BX23:BZ1048576 BX2:BX22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BY21:CA22 BY2:BZ20 BX23:BZ1048576 BX2:BX22" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"y, n, m"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB1048576 Y2:Y1048576 AE2:AE1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB1048576 Y2:Y1048576 AE2:AE1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"greater than, minimum, less than, maximum, average"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2:BK1048576 BH2:BH1048576 AD2:AD1048576 AG2:AG1048576 BB2:BB1048576 X2:X1048576 AJ2:AJ1048576 AY2:AY1048576 AV2:AV1048576 AS2:AS1048576 AP2:AP1048576 AM2:AM1048576 AA2:AA1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2:BK1048576 BH2:BH1048576 AD2:AD1048576 AG2:AG1048576 BB2:BB1048576 X2:X1048576 AJ2:AJ1048576 AY2:AY1048576 AV2:AV1048576 AS2:AS1048576 AP2:AP1048576 AM2:AM1048576 AA2:AA1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"release, measure, not stated"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M86:M1048576 M2:M43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M86:M1048576 M2:M43" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"adherence, density, immuno, enzymatic, not stated"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P86:P1048576 P2:P43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P86:P1048576 P2:P43" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"alpha-MEM, ns, IMEM, chemically defined, PlasmaLyte, commercial, DMEM, MEM, StemMACS, xeno-free"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="P44:P85">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="P44:P85" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"alpha-MEM,ns,IMEM,chemically defined,PlasmaLyte,commercial,DMEM,MEM,StemMACS,xeno-free"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M44:M85">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M44:M85" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"adherence,density,immuno,enzymatic,not stated"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AT2:AT1048576 AQ2:AQ1048576 AN2:AN1048576 AK2:AK1048576 AH2:AH1048576 AZ2:AZ1048576 AW2:AW1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AT2:AT1048576 AQ2:AQ1048576 AN2:AN1048576 AK2:AK1048576 AH2:AH1048576 AZ2:AZ1048576 AW2:AW1048576" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>"average, greater than, minimum, less than, maximum"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"cutaneous, intraarterial, intraarticular, intracardiac, intracavernous, intracoronary, intramuscular, intranasal, intraosseous, intraperitoneal, intrathecal, intravenous, intravitreous,implant, local injection, periodontal, subcutaneous, topical"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>"multipotent stromal, stromal, stem, regenerative, other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R1048576" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>"auto, allo, commercial, both"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S1048576" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>"male, female, both, not stated"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T1048576" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>"neonate, adult,ns"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{00000000-0002-0000-0000-00000D000000}">
       <formula1>"commercial, national govt, regional govt, other grant, mix, none, NS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-0000-00000E000000}">
       <formula1>"immune, differentiation, paracrine, NS, ?, multi"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF2:BF1048576 BI2:BI1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF2:BF1048576 BI2:BI1048576" xr:uid="{00000000-0002-0000-0000-00000F000000}">
       <formula1>"average, maximum, greater than, minimum, less than"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U1048576" xr:uid="{00000000-0002-0000-0000-000010000000}">
       <formula1>"y, n, s, o, t"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0000-000011000000}">
       <formula1>"I, I/IIa, IIa, II, IIb, III"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1048576" xr:uid="{00000000-0002-0000-0000-000012000000}">
       <formula1>"minimum, less than, maximum, greater than, average"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BN2:BN1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BN2:BN1048576" xr:uid="{00000000-0002-0000-0000-000013000000}">
       <formula1>"measure, release, non stated"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BL2:BL1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BL2:BL1048576" xr:uid="{00000000-0002-0000-0000-000014000000}">
       <formula1>"less than, minimum, maximum, greater than, average"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BO2:BO1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BO2:BO1048576" xr:uid="{00000000-0002-0000-0000-000015000000}">
       <formula1>"average, greater than, maximum, less than, minimum"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{00000000-0002-0000-0000-000016000000}">
       <formula1>"NS, bone marrow, adipose, wharton's jelly, umbilical cord, cord blood"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N1048576" xr:uid="{00000000-0002-0000-0000-000017000000}">
       <formula1>"autologous, fbs, ns, human ab"</formula1>
     </dataValidation>
   </dataValidations>
@@ -18615,7 +18651,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18623,26 +18659,26 @@
       <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="16"/>
-    <col min="2" max="2" width="8.85546875" style="135"/>
-    <col min="3" max="10" width="8.85546875" style="16"/>
-    <col min="11" max="11" width="8.85546875" style="52"/>
-    <col min="12" max="12" width="8.85546875" style="16"/>
-    <col min="13" max="13" width="8.85546875" style="135"/>
-    <col min="14" max="15" width="8.85546875" style="16"/>
-    <col min="16" max="16" width="8.85546875" style="80"/>
-    <col min="17" max="19" width="8.85546875" style="16"/>
-    <col min="20" max="20" width="8.85546875" style="80"/>
-    <col min="21" max="21" width="8.85546875" style="16"/>
-    <col min="22" max="23" width="14.140625" style="80" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="51.42578125" style="16" customWidth="1"/>
-    <col min="26" max="16384" width="8.85546875" style="16"/>
+    <col min="1" max="1" width="8.88671875" style="16"/>
+    <col min="2" max="2" width="8.88671875" style="135"/>
+    <col min="3" max="10" width="8.88671875" style="16"/>
+    <col min="11" max="11" width="8.88671875" style="52"/>
+    <col min="12" max="12" width="8.88671875" style="16"/>
+    <col min="13" max="13" width="8.88671875" style="135"/>
+    <col min="14" max="15" width="8.88671875" style="16"/>
+    <col min="16" max="16" width="8.88671875" style="80"/>
+    <col min="17" max="19" width="8.88671875" style="16"/>
+    <col min="20" max="20" width="8.88671875" style="80"/>
+    <col min="21" max="21" width="8.88671875" style="16"/>
+    <col min="22" max="23" width="14.109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="51.44140625" style="16" customWidth="1"/>
+    <col min="26" max="16384" width="8.88671875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" s="19" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>261</v>
       </c>
@@ -18713,7 +18749,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:25" s="19" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="16">
         <v>6</v>
@@ -20503,7 +20539,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="55" spans="1:25" s="52" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" s="52" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A55" s="52">
         <v>44</v>
       </c>
@@ -22237,16 +22273,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -22269,27 +22305,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z85"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="57.5703125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="43.5703125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="33.5703125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="57.5546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="43.5546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="33.5546875" style="6" customWidth="1"/>
     <col min="7" max="7" width="81" style="27" customWidth="1"/>
     <col min="8" max="8" width="20" style="5" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="5"/>
+    <col min="9" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="94" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="94" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="90" t="s">
         <v>8</v>
       </c>
@@ -22312,7 +22348,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -22335,7 +22371,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -22358,7 +22394,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -22381,7 +22417,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -22404,7 +22440,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -22427,7 +22463,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -22450,7 +22486,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -22473,7 +22509,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -22496,7 +22532,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -22519,7 +22555,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -22542,7 +22578,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -22565,7 +22601,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -22588,7 +22624,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -22611,7 +22647,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -22634,7 +22670,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="40.799999999999997" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -22657,7 +22693,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -22680,7 +22716,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="29" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="29" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" s="28">
         <v>17</v>
       </c>
@@ -22703,7 +22739,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="33" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="33" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A19" s="32">
         <v>18</v>
       </c>
@@ -22726,7 +22762,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="33" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="33" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="32">
         <v>19</v>
       </c>
@@ -22749,7 +22785,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="36" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="36" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A21" s="42">
         <v>20</v>
       </c>
@@ -22770,7 +22806,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -22793,7 +22829,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -22816,7 +22852,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -22839,7 +22875,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -22862,7 +22898,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -22885,7 +22921,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -22908,7 +22944,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -22931,7 +22967,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -22954,7 +22990,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -22977,7 +23013,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -23000,7 +23036,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>31</v>
       </c>
@@ -23023,7 +23059,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>32</v>
       </c>
@@ -23046,7 +23082,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>33</v>
       </c>
@@ -23069,7 +23105,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>34</v>
       </c>
@@ -23092,7 +23128,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>35</v>
       </c>
@@ -23115,7 +23151,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>36</v>
       </c>
@@ -23138,7 +23174,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="38" spans="1:26" s="3" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" s="3" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -23161,7 +23197,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>38</v>
       </c>
@@ -23184,7 +23220,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -23207,7 +23243,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:26" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>40</v>
       </c>
@@ -23230,7 +23266,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:26" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <v>41</v>
       </c>
@@ -23253,7 +23289,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="43" spans="1:26" ht="45" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26" ht="43.2" x14ac:dyDescent="0.2">
       <c r="A43" s="89">
         <v>42</v>
       </c>
@@ -23279,7 +23315,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="44" spans="1:26" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A44" s="89">
         <v>43</v>
       </c>
@@ -23321,7 +23357,7 @@
       <c r="Y44" s="85"/>
       <c r="Z44" s="85"/>
     </row>
-    <row r="45" spans="1:26" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" s="86" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="89">
         <v>44</v>
       </c>
@@ -23363,7 +23399,7 @@
       <c r="Y45" s="85"/>
       <c r="Z45" s="85"/>
     </row>
-    <row r="46" spans="1:26" s="86" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" s="86" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="81">
         <v>45</v>
       </c>
@@ -23405,7 +23441,7 @@
       <c r="Y46" s="85"/>
       <c r="Z46" s="85"/>
     </row>
-    <row r="47" spans="1:26" s="86" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" s="86" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A47" s="81">
         <v>46</v>
       </c>
@@ -23447,7 +23483,7 @@
       <c r="Y47" s="85"/>
       <c r="Z47" s="85"/>
     </row>
-    <row r="48" spans="1:26" s="86" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A48" s="81">
         <v>47</v>
       </c>
@@ -23489,7 +23525,7 @@
       <c r="Y48" s="85"/>
       <c r="Z48" s="85"/>
     </row>
-    <row r="49" spans="1:26" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" s="86" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="81">
         <v>48</v>
       </c>
@@ -23531,7 +23567,7 @@
       <c r="Y49" s="85"/>
       <c r="Z49" s="85"/>
     </row>
-    <row r="50" spans="1:26" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" s="86" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="81">
         <v>49</v>
       </c>
@@ -23573,7 +23609,7 @@
       <c r="Y50" s="85"/>
       <c r="Z50" s="85"/>
     </row>
-    <row r="51" spans="1:26" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" s="86" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="81">
         <v>50</v>
       </c>
@@ -23615,7 +23651,7 @@
       <c r="Y51" s="85"/>
       <c r="Z51" s="85"/>
     </row>
-    <row r="52" spans="1:26" s="86" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A52" s="81">
         <v>51</v>
       </c>
@@ -23657,7 +23693,7 @@
       <c r="Y52" s="85"/>
       <c r="Z52" s="85"/>
     </row>
-    <row r="53" spans="1:26" s="86" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A53" s="81">
         <v>52</v>
       </c>
@@ -23699,7 +23735,7 @@
       <c r="Y53" s="85"/>
       <c r="Z53" s="85"/>
     </row>
-    <row r="54" spans="1:26" s="86" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A54" s="81">
         <v>53</v>
       </c>
@@ -23741,7 +23777,7 @@
       <c r="Y54" s="85"/>
       <c r="Z54" s="85"/>
     </row>
-    <row r="55" spans="1:26" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" s="86" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="81">
         <v>54</v>
       </c>
@@ -23783,7 +23819,7 @@
       <c r="Y55" s="85"/>
       <c r="Z55" s="85"/>
     </row>
-    <row r="56" spans="1:26" s="86" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" s="86" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A56" s="81">
         <v>55</v>
       </c>
@@ -23825,7 +23861,7 @@
       <c r="Y56" s="85"/>
       <c r="Z56" s="85"/>
     </row>
-    <row r="57" spans="1:26" s="86" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" s="86" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A57" s="81">
         <v>56</v>
       </c>
@@ -23867,7 +23903,7 @@
       <c r="Y57" s="85"/>
       <c r="Z57" s="85"/>
     </row>
-    <row r="58" spans="1:26" s="86" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A58" s="81">
         <v>57</v>
       </c>
@@ -23909,7 +23945,7 @@
       <c r="Y58" s="85"/>
       <c r="Z58" s="85"/>
     </row>
-    <row r="59" spans="1:26" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A59" s="81">
         <v>58</v>
       </c>
@@ -23951,7 +23987,7 @@
       <c r="Y59" s="85"/>
       <c r="Z59" s="85"/>
     </row>
-    <row r="60" spans="1:26" s="86" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A60" s="81">
         <v>59</v>
       </c>
@@ -23993,7 +24029,7 @@
       <c r="Y60" s="85"/>
       <c r="Z60" s="85"/>
     </row>
-    <row r="61" spans="1:26" s="86" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A61" s="81">
         <v>60</v>
       </c>
@@ -24035,7 +24071,7 @@
       <c r="Y61" s="85"/>
       <c r="Z61" s="85"/>
     </row>
-    <row r="62" spans="1:26" s="86" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A62" s="81">
         <v>61</v>
       </c>
@@ -24075,7 +24111,7 @@
       <c r="Y62" s="85"/>
       <c r="Z62" s="85"/>
     </row>
-    <row r="63" spans="1:26" s="86" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" s="86" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="81">
         <v>62</v>
       </c>
@@ -24117,7 +24153,7 @@
       <c r="Y63" s="85"/>
       <c r="Z63" s="85"/>
     </row>
-    <row r="64" spans="1:26" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" s="86" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="81">
         <v>63</v>
       </c>
@@ -24157,7 +24193,7 @@
       <c r="Y64" s="85"/>
       <c r="Z64" s="85"/>
     </row>
-    <row r="65" spans="1:26" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A65" s="81">
         <v>64</v>
       </c>
@@ -24197,7 +24233,7 @@
       <c r="Y65" s="85"/>
       <c r="Z65" s="85"/>
     </row>
-    <row r="66" spans="1:26" s="86" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A66" s="81">
         <v>65</v>
       </c>
@@ -24237,7 +24273,7 @@
       <c r="Y66" s="85"/>
       <c r="Z66" s="85"/>
     </row>
-    <row r="67" spans="1:26" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" s="86" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A67" s="81">
         <v>66</v>
       </c>
@@ -24277,7 +24313,7 @@
       <c r="Y67" s="85"/>
       <c r="Z67" s="85"/>
     </row>
-    <row r="68" spans="1:26" s="86" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A68" s="81">
         <v>67</v>
       </c>
@@ -24317,7 +24353,7 @@
       <c r="Y68" s="85"/>
       <c r="Z68" s="85"/>
     </row>
-    <row r="69" spans="1:26" s="86" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" s="86" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A69" s="81">
         <v>68</v>
       </c>
@@ -24357,7 +24393,7 @@
       <c r="Y69" s="85"/>
       <c r="Z69" s="85"/>
     </row>
-    <row r="70" spans="1:26" s="86" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A70" s="81">
         <v>69</v>
       </c>
@@ -24397,7 +24433,7 @@
       <c r="Y70" s="85"/>
       <c r="Z70" s="85"/>
     </row>
-    <row r="71" spans="1:26" s="86" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" s="86" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A71" s="81">
         <v>70</v>
       </c>
@@ -24439,7 +24475,7 @@
       <c r="Y71" s="85"/>
       <c r="Z71" s="85"/>
     </row>
-    <row r="72" spans="1:26" s="86" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" s="86" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A72" s="81">
         <v>71</v>
       </c>
@@ -24479,7 +24515,7 @@
       <c r="Y72" s="85"/>
       <c r="Z72" s="85"/>
     </row>
-    <row r="73" spans="1:26" s="86" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" s="86" customFormat="1" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A73" s="81">
         <v>72</v>
       </c>
@@ -24519,7 +24555,7 @@
       <c r="Y73" s="85"/>
       <c r="Z73" s="85"/>
     </row>
-    <row r="74" spans="1:26" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A74" s="81">
         <v>73</v>
       </c>
@@ -24559,7 +24595,7 @@
       <c r="Y74" s="85"/>
       <c r="Z74" s="85"/>
     </row>
-    <row r="75" spans="1:26" s="86" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A75" s="81">
         <v>74</v>
       </c>
@@ -24599,7 +24635,7 @@
       <c r="Y75" s="85"/>
       <c r="Z75" s="85"/>
     </row>
-    <row r="76" spans="1:26" s="86" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" s="86" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A76" s="81">
         <v>75</v>
       </c>
@@ -24639,7 +24675,7 @@
       <c r="Y76" s="85"/>
       <c r="Z76" s="85"/>
     </row>
-    <row r="77" spans="1:26" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A77" s="81">
         <v>76</v>
       </c>
@@ -24681,7 +24717,7 @@
       <c r="Y77" s="85"/>
       <c r="Z77" s="85"/>
     </row>
-    <row r="78" spans="1:26" s="86" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" s="86" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A78" s="81">
         <v>77</v>
       </c>
@@ -24723,7 +24759,7 @@
       <c r="Y78" s="85"/>
       <c r="Z78" s="85"/>
     </row>
-    <row r="79" spans="1:26" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A79" s="81">
         <v>78</v>
       </c>
@@ -24765,7 +24801,7 @@
       <c r="Y79" s="85"/>
       <c r="Z79" s="85"/>
     </row>
-    <row r="80" spans="1:26" s="86" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" s="86" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A80" s="81">
         <v>79</v>
       </c>
@@ -24807,7 +24843,7 @@
       <c r="Y80" s="85"/>
       <c r="Z80" s="85"/>
     </row>
-    <row r="81" spans="1:26" s="86" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" s="86" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A81" s="81">
         <v>80</v>
       </c>
@@ -24849,7 +24885,7 @@
       <c r="Y81" s="85"/>
       <c r="Z81" s="85"/>
     </row>
-    <row r="82" spans="1:26" s="86" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A82" s="81">
         <v>81</v>
       </c>
@@ -24891,7 +24927,7 @@
       <c r="Y82" s="85"/>
       <c r="Z82" s="85"/>
     </row>
-    <row r="83" spans="1:26" s="86" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" s="86" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A83" s="81">
         <v>82</v>
       </c>
@@ -24933,7 +24969,7 @@
       <c r="Y83" s="85"/>
       <c r="Z83" s="85"/>
     </row>
-    <row r="84" spans="1:26" s="86" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A84" s="81">
         <v>83</v>
       </c>
@@ -24975,7 +25011,7 @@
       <c r="Y84" s="85"/>
       <c r="Z84" s="85"/>
     </row>
-    <row r="85" spans="1:26" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" s="86" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A85" s="81">
         <v>84</v>
       </c>
@@ -25018,167 +25054,167 @@
       <c r="Z85" s="85"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A88">
-    <sortState ref="A2:H99">
+  <autoFilter ref="A1:A88" xr:uid="{00000000-0009-0000-0000-000003000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H99">
       <sortCondition ref="A1:A99"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="F2" r:id="rId3"/>
-    <hyperlink ref="F3" r:id="rId4"/>
-    <hyperlink ref="F4" r:id="rId5"/>
-    <hyperlink ref="F5" r:id="rId6"/>
-    <hyperlink ref="F6" r:id="rId7"/>
-    <hyperlink ref="G6" r:id="rId8"/>
-    <hyperlink ref="G7" r:id="rId9"/>
-    <hyperlink ref="F7" r:id="rId10"/>
-    <hyperlink ref="G8" r:id="rId11"/>
-    <hyperlink ref="F8" r:id="rId12"/>
-    <hyperlink ref="F9" r:id="rId13"/>
-    <hyperlink ref="G10" r:id="rId14" location="pdf-link"/>
-    <hyperlink ref="G9" r:id="rId15"/>
-    <hyperlink ref="F10" r:id="rId16"/>
-    <hyperlink ref="G11" r:id="rId17"/>
-    <hyperlink ref="F11" r:id="rId18"/>
-    <hyperlink ref="G12" r:id="rId19"/>
-    <hyperlink ref="F12" r:id="rId20"/>
-    <hyperlink ref="G13" r:id="rId21"/>
-    <hyperlink ref="F13" r:id="rId22"/>
-    <hyperlink ref="G14" r:id="rId23"/>
-    <hyperlink ref="F14" r:id="rId24"/>
-    <hyperlink ref="G15" r:id="rId25"/>
-    <hyperlink ref="G5" r:id="rId26"/>
-    <hyperlink ref="G4" r:id="rId27"/>
-    <hyperlink ref="G16" r:id="rId28"/>
-    <hyperlink ref="F16" r:id="rId29"/>
-    <hyperlink ref="G17" r:id="rId30"/>
-    <hyperlink ref="F17" r:id="rId31"/>
-    <hyperlink ref="G18" r:id="rId32"/>
-    <hyperlink ref="G19" r:id="rId33"/>
-    <hyperlink ref="G20" r:id="rId34"/>
-    <hyperlink ref="E21" r:id="rId35" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6301165/"/>
-    <hyperlink ref="G21" r:id="rId36"/>
-    <hyperlink ref="G22" r:id="rId37"/>
-    <hyperlink ref="G23" r:id="rId38"/>
-    <hyperlink ref="G24" r:id="rId39"/>
-    <hyperlink ref="G25" r:id="rId40"/>
-    <hyperlink ref="G26" r:id="rId41"/>
-    <hyperlink ref="F22" r:id="rId42"/>
-    <hyperlink ref="F23" r:id="rId43"/>
-    <hyperlink ref="F24" r:id="rId44"/>
-    <hyperlink ref="F25" r:id="rId45"/>
-    <hyperlink ref="F26" r:id="rId46"/>
-    <hyperlink ref="F18" r:id="rId47"/>
-    <hyperlink ref="F19" r:id="rId48"/>
-    <hyperlink ref="F20" r:id="rId49"/>
-    <hyperlink ref="G27" r:id="rId50"/>
-    <hyperlink ref="F27" r:id="rId51"/>
-    <hyperlink ref="G28" r:id="rId52"/>
-    <hyperlink ref="F28" r:id="rId53"/>
-    <hyperlink ref="G29" r:id="rId54"/>
-    <hyperlink ref="F29" r:id="rId55"/>
-    <hyperlink ref="G30" r:id="rId56"/>
-    <hyperlink ref="F30" r:id="rId57"/>
-    <hyperlink ref="G31" r:id="rId58"/>
-    <hyperlink ref="F31" r:id="rId59"/>
-    <hyperlink ref="G32" r:id="rId60"/>
-    <hyperlink ref="F32" r:id="rId61"/>
-    <hyperlink ref="G33" r:id="rId62"/>
-    <hyperlink ref="F34" r:id="rId63"/>
-    <hyperlink ref="F33" r:id="rId64"/>
-    <hyperlink ref="G34" r:id="rId65"/>
-    <hyperlink ref="G35" r:id="rId66"/>
-    <hyperlink ref="F35" r:id="rId67"/>
-    <hyperlink ref="G36" r:id="rId68"/>
-    <hyperlink ref="F36" r:id="rId69"/>
-    <hyperlink ref="G37" r:id="rId70"/>
-    <hyperlink ref="F37" r:id="rId71"/>
-    <hyperlink ref="G38" r:id="rId72"/>
-    <hyperlink ref="F38" r:id="rId73"/>
-    <hyperlink ref="G39" r:id="rId74"/>
-    <hyperlink ref="F39" r:id="rId75"/>
-    <hyperlink ref="G40" r:id="rId76"/>
-    <hyperlink ref="F40" r:id="rId77"/>
-    <hyperlink ref="G41" r:id="rId78"/>
-    <hyperlink ref="F41" r:id="rId79"/>
-    <hyperlink ref="G42" r:id="rId80"/>
-    <hyperlink ref="F42" r:id="rId81"/>
-    <hyperlink ref="G43" r:id="rId82" location="pdf-link"/>
-    <hyperlink ref="F44" r:id="rId83"/>
-    <hyperlink ref="F43" r:id="rId84"/>
-    <hyperlink ref="G44" r:id="rId85"/>
-    <hyperlink ref="F45" r:id="rId86"/>
-    <hyperlink ref="G45" r:id="rId87"/>
-    <hyperlink ref="F46" r:id="rId88"/>
-    <hyperlink ref="G46" r:id="rId89" location="Sec11" display="https://link.springer.com/article/10.1007%2Fs00384-012-1581-9 - Sec11"/>
-    <hyperlink ref="F47" r:id="rId90"/>
-    <hyperlink ref="G47" r:id="rId91"/>
-    <hyperlink ref="G48" r:id="rId92"/>
-    <hyperlink ref="F48" r:id="rId93"/>
-    <hyperlink ref="G49" r:id="rId94"/>
-    <hyperlink ref="F49" r:id="rId95"/>
-    <hyperlink ref="G50" r:id="rId96"/>
-    <hyperlink ref="F50" r:id="rId97"/>
-    <hyperlink ref="G51" r:id="rId98"/>
-    <hyperlink ref="F51" r:id="rId99"/>
-    <hyperlink ref="G52" r:id="rId100"/>
-    <hyperlink ref="F52" r:id="rId101"/>
-    <hyperlink ref="G53" r:id="rId102"/>
-    <hyperlink ref="F53" r:id="rId103"/>
-    <hyperlink ref="G54" r:id="rId104"/>
-    <hyperlink ref="F54" r:id="rId105"/>
-    <hyperlink ref="F15" r:id="rId106"/>
-    <hyperlink ref="G55" r:id="rId107"/>
-    <hyperlink ref="F55" r:id="rId108"/>
-    <hyperlink ref="G56" r:id="rId109"/>
-    <hyperlink ref="F56" r:id="rId110"/>
-    <hyperlink ref="G57" r:id="rId111"/>
-    <hyperlink ref="F57" r:id="rId112"/>
-    <hyperlink ref="G58" r:id="rId113"/>
-    <hyperlink ref="F58" r:id="rId114"/>
-    <hyperlink ref="G59" r:id="rId115"/>
-    <hyperlink ref="F59" r:id="rId116"/>
-    <hyperlink ref="F60" r:id="rId117"/>
-    <hyperlink ref="G60" r:id="rId118"/>
-    <hyperlink ref="F61" r:id="rId119"/>
-    <hyperlink ref="F62" r:id="rId120"/>
-    <hyperlink ref="F63" r:id="rId121"/>
-    <hyperlink ref="F64" r:id="rId122"/>
-    <hyperlink ref="F65" r:id="rId123"/>
-    <hyperlink ref="F66" r:id="rId124"/>
-    <hyperlink ref="F67" r:id="rId125"/>
-    <hyperlink ref="F68" r:id="rId126"/>
-    <hyperlink ref="F69" r:id="rId127"/>
-    <hyperlink ref="F70" r:id="rId128"/>
-    <hyperlink ref="F71" r:id="rId129"/>
-    <hyperlink ref="F72" r:id="rId130"/>
-    <hyperlink ref="F73" r:id="rId131"/>
-    <hyperlink ref="F74" r:id="rId132"/>
-    <hyperlink ref="F75" r:id="rId133"/>
-    <hyperlink ref="F76" r:id="rId134"/>
-    <hyperlink ref="F77" r:id="rId135"/>
-    <hyperlink ref="F78" r:id="rId136"/>
-    <hyperlink ref="F79" r:id="rId137"/>
-    <hyperlink ref="F80" r:id="rId138"/>
-    <hyperlink ref="F81" r:id="rId139"/>
-    <hyperlink ref="F82" r:id="rId140"/>
-    <hyperlink ref="F83" r:id="rId141"/>
-    <hyperlink ref="F84" r:id="rId142"/>
-    <hyperlink ref="F85" r:id="rId143"/>
-    <hyperlink ref="G77" r:id="rId144" location="s0130" display="https://www.sciencedirect.com/science/article/pii/S1465324916303772?via%3Dihub - s0130"/>
-    <hyperlink ref="G78" r:id="rId145"/>
-    <hyperlink ref="G61" r:id="rId146"/>
-    <hyperlink ref="G79" r:id="rId147"/>
-    <hyperlink ref="G80" r:id="rId148"/>
-    <hyperlink ref="G81" r:id="rId149"/>
-    <hyperlink ref="G82" r:id="rId150"/>
-    <hyperlink ref="G84" r:id="rId151"/>
-    <hyperlink ref="G83" r:id="rId152"/>
-    <hyperlink ref="G85" r:id="rId153"/>
-    <hyperlink ref="G63" r:id="rId154"/>
-    <hyperlink ref="G71" r:id="rId155"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="F3" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="F5" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="F6" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="G6" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="G7" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="F7" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
+    <hyperlink ref="G8" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
+    <hyperlink ref="F8" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
+    <hyperlink ref="F9" r:id="rId13" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
+    <hyperlink ref="G10" r:id="rId14" location="pdf-link" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
+    <hyperlink ref="G9" r:id="rId15" xr:uid="{00000000-0004-0000-0300-00000E000000}"/>
+    <hyperlink ref="F10" r:id="rId16" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
+    <hyperlink ref="G11" r:id="rId17" xr:uid="{00000000-0004-0000-0300-000010000000}"/>
+    <hyperlink ref="F11" r:id="rId18" xr:uid="{00000000-0004-0000-0300-000011000000}"/>
+    <hyperlink ref="G12" r:id="rId19" xr:uid="{00000000-0004-0000-0300-000012000000}"/>
+    <hyperlink ref="F12" r:id="rId20" xr:uid="{00000000-0004-0000-0300-000013000000}"/>
+    <hyperlink ref="G13" r:id="rId21" xr:uid="{00000000-0004-0000-0300-000014000000}"/>
+    <hyperlink ref="F13" r:id="rId22" xr:uid="{00000000-0004-0000-0300-000015000000}"/>
+    <hyperlink ref="G14" r:id="rId23" xr:uid="{00000000-0004-0000-0300-000016000000}"/>
+    <hyperlink ref="F14" r:id="rId24" xr:uid="{00000000-0004-0000-0300-000017000000}"/>
+    <hyperlink ref="G15" r:id="rId25" xr:uid="{00000000-0004-0000-0300-000018000000}"/>
+    <hyperlink ref="G5" r:id="rId26" xr:uid="{00000000-0004-0000-0300-000019000000}"/>
+    <hyperlink ref="G4" r:id="rId27" xr:uid="{00000000-0004-0000-0300-00001A000000}"/>
+    <hyperlink ref="G16" r:id="rId28" xr:uid="{00000000-0004-0000-0300-00001B000000}"/>
+    <hyperlink ref="F16" r:id="rId29" xr:uid="{00000000-0004-0000-0300-00001C000000}"/>
+    <hyperlink ref="G17" r:id="rId30" xr:uid="{00000000-0004-0000-0300-00001D000000}"/>
+    <hyperlink ref="F17" r:id="rId31" xr:uid="{00000000-0004-0000-0300-00001E000000}"/>
+    <hyperlink ref="G18" r:id="rId32" xr:uid="{00000000-0004-0000-0300-00001F000000}"/>
+    <hyperlink ref="G19" r:id="rId33" xr:uid="{00000000-0004-0000-0300-000020000000}"/>
+    <hyperlink ref="G20" r:id="rId34" xr:uid="{00000000-0004-0000-0300-000021000000}"/>
+    <hyperlink ref="E21" r:id="rId35" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6301165/" xr:uid="{00000000-0004-0000-0300-000022000000}"/>
+    <hyperlink ref="G21" r:id="rId36" xr:uid="{00000000-0004-0000-0300-000023000000}"/>
+    <hyperlink ref="G22" r:id="rId37" xr:uid="{00000000-0004-0000-0300-000024000000}"/>
+    <hyperlink ref="G23" r:id="rId38" xr:uid="{00000000-0004-0000-0300-000025000000}"/>
+    <hyperlink ref="G24" r:id="rId39" xr:uid="{00000000-0004-0000-0300-000026000000}"/>
+    <hyperlink ref="G25" r:id="rId40" xr:uid="{00000000-0004-0000-0300-000027000000}"/>
+    <hyperlink ref="G26" r:id="rId41" xr:uid="{00000000-0004-0000-0300-000028000000}"/>
+    <hyperlink ref="F22" r:id="rId42" xr:uid="{00000000-0004-0000-0300-000029000000}"/>
+    <hyperlink ref="F23" r:id="rId43" xr:uid="{00000000-0004-0000-0300-00002A000000}"/>
+    <hyperlink ref="F24" r:id="rId44" xr:uid="{00000000-0004-0000-0300-00002B000000}"/>
+    <hyperlink ref="F25" r:id="rId45" xr:uid="{00000000-0004-0000-0300-00002C000000}"/>
+    <hyperlink ref="F26" r:id="rId46" xr:uid="{00000000-0004-0000-0300-00002D000000}"/>
+    <hyperlink ref="F18" r:id="rId47" xr:uid="{00000000-0004-0000-0300-00002E000000}"/>
+    <hyperlink ref="F19" r:id="rId48" xr:uid="{00000000-0004-0000-0300-00002F000000}"/>
+    <hyperlink ref="F20" r:id="rId49" xr:uid="{00000000-0004-0000-0300-000030000000}"/>
+    <hyperlink ref="G27" r:id="rId50" xr:uid="{00000000-0004-0000-0300-000031000000}"/>
+    <hyperlink ref="F27" r:id="rId51" xr:uid="{00000000-0004-0000-0300-000032000000}"/>
+    <hyperlink ref="G28" r:id="rId52" xr:uid="{00000000-0004-0000-0300-000033000000}"/>
+    <hyperlink ref="F28" r:id="rId53" xr:uid="{00000000-0004-0000-0300-000034000000}"/>
+    <hyperlink ref="G29" r:id="rId54" xr:uid="{00000000-0004-0000-0300-000035000000}"/>
+    <hyperlink ref="F29" r:id="rId55" xr:uid="{00000000-0004-0000-0300-000036000000}"/>
+    <hyperlink ref="G30" r:id="rId56" xr:uid="{00000000-0004-0000-0300-000037000000}"/>
+    <hyperlink ref="F30" r:id="rId57" xr:uid="{00000000-0004-0000-0300-000038000000}"/>
+    <hyperlink ref="G31" r:id="rId58" xr:uid="{00000000-0004-0000-0300-000039000000}"/>
+    <hyperlink ref="F31" r:id="rId59" xr:uid="{00000000-0004-0000-0300-00003A000000}"/>
+    <hyperlink ref="G32" r:id="rId60" xr:uid="{00000000-0004-0000-0300-00003B000000}"/>
+    <hyperlink ref="F32" r:id="rId61" xr:uid="{00000000-0004-0000-0300-00003C000000}"/>
+    <hyperlink ref="G33" r:id="rId62" xr:uid="{00000000-0004-0000-0300-00003D000000}"/>
+    <hyperlink ref="F34" r:id="rId63" xr:uid="{00000000-0004-0000-0300-00003E000000}"/>
+    <hyperlink ref="F33" r:id="rId64" xr:uid="{00000000-0004-0000-0300-00003F000000}"/>
+    <hyperlink ref="G34" r:id="rId65" xr:uid="{00000000-0004-0000-0300-000040000000}"/>
+    <hyperlink ref="G35" r:id="rId66" xr:uid="{00000000-0004-0000-0300-000041000000}"/>
+    <hyperlink ref="F35" r:id="rId67" xr:uid="{00000000-0004-0000-0300-000042000000}"/>
+    <hyperlink ref="G36" r:id="rId68" xr:uid="{00000000-0004-0000-0300-000043000000}"/>
+    <hyperlink ref="F36" r:id="rId69" xr:uid="{00000000-0004-0000-0300-000044000000}"/>
+    <hyperlink ref="G37" r:id="rId70" xr:uid="{00000000-0004-0000-0300-000045000000}"/>
+    <hyperlink ref="F37" r:id="rId71" xr:uid="{00000000-0004-0000-0300-000046000000}"/>
+    <hyperlink ref="G38" r:id="rId72" xr:uid="{00000000-0004-0000-0300-000047000000}"/>
+    <hyperlink ref="F38" r:id="rId73" xr:uid="{00000000-0004-0000-0300-000048000000}"/>
+    <hyperlink ref="G39" r:id="rId74" xr:uid="{00000000-0004-0000-0300-000049000000}"/>
+    <hyperlink ref="F39" r:id="rId75" xr:uid="{00000000-0004-0000-0300-00004A000000}"/>
+    <hyperlink ref="G40" r:id="rId76" xr:uid="{00000000-0004-0000-0300-00004B000000}"/>
+    <hyperlink ref="F40" r:id="rId77" xr:uid="{00000000-0004-0000-0300-00004C000000}"/>
+    <hyperlink ref="G41" r:id="rId78" xr:uid="{00000000-0004-0000-0300-00004D000000}"/>
+    <hyperlink ref="F41" r:id="rId79" xr:uid="{00000000-0004-0000-0300-00004E000000}"/>
+    <hyperlink ref="G42" r:id="rId80" xr:uid="{00000000-0004-0000-0300-00004F000000}"/>
+    <hyperlink ref="F42" r:id="rId81" xr:uid="{00000000-0004-0000-0300-000050000000}"/>
+    <hyperlink ref="G43" r:id="rId82" location="pdf-link" xr:uid="{00000000-0004-0000-0300-000051000000}"/>
+    <hyperlink ref="F44" r:id="rId83" xr:uid="{00000000-0004-0000-0300-000052000000}"/>
+    <hyperlink ref="F43" r:id="rId84" xr:uid="{00000000-0004-0000-0300-000053000000}"/>
+    <hyperlink ref="G44" r:id="rId85" xr:uid="{00000000-0004-0000-0300-000054000000}"/>
+    <hyperlink ref="F45" r:id="rId86" xr:uid="{00000000-0004-0000-0300-000055000000}"/>
+    <hyperlink ref="G45" r:id="rId87" xr:uid="{00000000-0004-0000-0300-000056000000}"/>
+    <hyperlink ref="F46" r:id="rId88" xr:uid="{00000000-0004-0000-0300-000057000000}"/>
+    <hyperlink ref="G46" r:id="rId89" location="Sec11" display="https://link.springer.com/article/10.1007%2Fs00384-012-1581-9 - Sec11" xr:uid="{00000000-0004-0000-0300-000058000000}"/>
+    <hyperlink ref="F47" r:id="rId90" xr:uid="{00000000-0004-0000-0300-000059000000}"/>
+    <hyperlink ref="G47" r:id="rId91" xr:uid="{00000000-0004-0000-0300-00005A000000}"/>
+    <hyperlink ref="G48" r:id="rId92" xr:uid="{00000000-0004-0000-0300-00005B000000}"/>
+    <hyperlink ref="F48" r:id="rId93" xr:uid="{00000000-0004-0000-0300-00005C000000}"/>
+    <hyperlink ref="G49" r:id="rId94" xr:uid="{00000000-0004-0000-0300-00005D000000}"/>
+    <hyperlink ref="F49" r:id="rId95" xr:uid="{00000000-0004-0000-0300-00005E000000}"/>
+    <hyperlink ref="G50" r:id="rId96" xr:uid="{00000000-0004-0000-0300-00005F000000}"/>
+    <hyperlink ref="F50" r:id="rId97" xr:uid="{00000000-0004-0000-0300-000060000000}"/>
+    <hyperlink ref="G51" r:id="rId98" xr:uid="{00000000-0004-0000-0300-000061000000}"/>
+    <hyperlink ref="F51" r:id="rId99" xr:uid="{00000000-0004-0000-0300-000062000000}"/>
+    <hyperlink ref="G52" r:id="rId100" xr:uid="{00000000-0004-0000-0300-000063000000}"/>
+    <hyperlink ref="F52" r:id="rId101" xr:uid="{00000000-0004-0000-0300-000064000000}"/>
+    <hyperlink ref="G53" r:id="rId102" xr:uid="{00000000-0004-0000-0300-000065000000}"/>
+    <hyperlink ref="F53" r:id="rId103" xr:uid="{00000000-0004-0000-0300-000066000000}"/>
+    <hyperlink ref="G54" r:id="rId104" xr:uid="{00000000-0004-0000-0300-000067000000}"/>
+    <hyperlink ref="F54" r:id="rId105" xr:uid="{00000000-0004-0000-0300-000068000000}"/>
+    <hyperlink ref="F15" r:id="rId106" xr:uid="{00000000-0004-0000-0300-000069000000}"/>
+    <hyperlink ref="G55" r:id="rId107" xr:uid="{00000000-0004-0000-0300-00006A000000}"/>
+    <hyperlink ref="F55" r:id="rId108" xr:uid="{00000000-0004-0000-0300-00006B000000}"/>
+    <hyperlink ref="G56" r:id="rId109" xr:uid="{00000000-0004-0000-0300-00006C000000}"/>
+    <hyperlink ref="F56" r:id="rId110" xr:uid="{00000000-0004-0000-0300-00006D000000}"/>
+    <hyperlink ref="G57" r:id="rId111" xr:uid="{00000000-0004-0000-0300-00006E000000}"/>
+    <hyperlink ref="F57" r:id="rId112" xr:uid="{00000000-0004-0000-0300-00006F000000}"/>
+    <hyperlink ref="G58" r:id="rId113" xr:uid="{00000000-0004-0000-0300-000070000000}"/>
+    <hyperlink ref="F58" r:id="rId114" xr:uid="{00000000-0004-0000-0300-000071000000}"/>
+    <hyperlink ref="G59" r:id="rId115" xr:uid="{00000000-0004-0000-0300-000072000000}"/>
+    <hyperlink ref="F59" r:id="rId116" xr:uid="{00000000-0004-0000-0300-000073000000}"/>
+    <hyperlink ref="F60" r:id="rId117" xr:uid="{00000000-0004-0000-0300-000074000000}"/>
+    <hyperlink ref="G60" r:id="rId118" xr:uid="{00000000-0004-0000-0300-000075000000}"/>
+    <hyperlink ref="F61" r:id="rId119" xr:uid="{00000000-0004-0000-0300-000076000000}"/>
+    <hyperlink ref="F62" r:id="rId120" xr:uid="{00000000-0004-0000-0300-000077000000}"/>
+    <hyperlink ref="F63" r:id="rId121" xr:uid="{00000000-0004-0000-0300-000078000000}"/>
+    <hyperlink ref="F64" r:id="rId122" xr:uid="{00000000-0004-0000-0300-000079000000}"/>
+    <hyperlink ref="F65" r:id="rId123" xr:uid="{00000000-0004-0000-0300-00007A000000}"/>
+    <hyperlink ref="F66" r:id="rId124" xr:uid="{00000000-0004-0000-0300-00007B000000}"/>
+    <hyperlink ref="F67" r:id="rId125" xr:uid="{00000000-0004-0000-0300-00007C000000}"/>
+    <hyperlink ref="F68" r:id="rId126" xr:uid="{00000000-0004-0000-0300-00007D000000}"/>
+    <hyperlink ref="F69" r:id="rId127" xr:uid="{00000000-0004-0000-0300-00007E000000}"/>
+    <hyperlink ref="F70" r:id="rId128" xr:uid="{00000000-0004-0000-0300-00007F000000}"/>
+    <hyperlink ref="F71" r:id="rId129" xr:uid="{00000000-0004-0000-0300-000080000000}"/>
+    <hyperlink ref="F72" r:id="rId130" xr:uid="{00000000-0004-0000-0300-000081000000}"/>
+    <hyperlink ref="F73" r:id="rId131" xr:uid="{00000000-0004-0000-0300-000082000000}"/>
+    <hyperlink ref="F74" r:id="rId132" xr:uid="{00000000-0004-0000-0300-000083000000}"/>
+    <hyperlink ref="F75" r:id="rId133" xr:uid="{00000000-0004-0000-0300-000084000000}"/>
+    <hyperlink ref="F76" r:id="rId134" xr:uid="{00000000-0004-0000-0300-000085000000}"/>
+    <hyperlink ref="F77" r:id="rId135" xr:uid="{00000000-0004-0000-0300-000086000000}"/>
+    <hyperlink ref="F78" r:id="rId136" xr:uid="{00000000-0004-0000-0300-000087000000}"/>
+    <hyperlink ref="F79" r:id="rId137" xr:uid="{00000000-0004-0000-0300-000088000000}"/>
+    <hyperlink ref="F80" r:id="rId138" xr:uid="{00000000-0004-0000-0300-000089000000}"/>
+    <hyperlink ref="F81" r:id="rId139" xr:uid="{00000000-0004-0000-0300-00008A000000}"/>
+    <hyperlink ref="F82" r:id="rId140" xr:uid="{00000000-0004-0000-0300-00008B000000}"/>
+    <hyperlink ref="F83" r:id="rId141" xr:uid="{00000000-0004-0000-0300-00008C000000}"/>
+    <hyperlink ref="F84" r:id="rId142" xr:uid="{00000000-0004-0000-0300-00008D000000}"/>
+    <hyperlink ref="F85" r:id="rId143" xr:uid="{00000000-0004-0000-0300-00008E000000}"/>
+    <hyperlink ref="G77" r:id="rId144" location="s0130" display="https://www.sciencedirect.com/science/article/pii/S1465324916303772?via%3Dihub - s0130" xr:uid="{00000000-0004-0000-0300-00008F000000}"/>
+    <hyperlink ref="G78" r:id="rId145" xr:uid="{00000000-0004-0000-0300-000090000000}"/>
+    <hyperlink ref="G61" r:id="rId146" xr:uid="{00000000-0004-0000-0300-000091000000}"/>
+    <hyperlink ref="G79" r:id="rId147" xr:uid="{00000000-0004-0000-0300-000092000000}"/>
+    <hyperlink ref="G80" r:id="rId148" xr:uid="{00000000-0004-0000-0300-000093000000}"/>
+    <hyperlink ref="G81" r:id="rId149" xr:uid="{00000000-0004-0000-0300-000094000000}"/>
+    <hyperlink ref="G82" r:id="rId150" xr:uid="{00000000-0004-0000-0300-000095000000}"/>
+    <hyperlink ref="G84" r:id="rId151" xr:uid="{00000000-0004-0000-0300-000096000000}"/>
+    <hyperlink ref="G83" r:id="rId152" xr:uid="{00000000-0004-0000-0300-000097000000}"/>
+    <hyperlink ref="G85" r:id="rId153" xr:uid="{00000000-0004-0000-0300-000098000000}"/>
+    <hyperlink ref="G63" r:id="rId154" xr:uid="{00000000-0004-0000-0300-000099000000}"/>
+    <hyperlink ref="G71" r:id="rId155" xr:uid="{00000000-0004-0000-0300-00009A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId156"/>
@@ -25186,23 +25222,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="51.85546875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="14.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="51.88671875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -25221,7 +25257,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="5" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>150</v>
       </c>
@@ -25244,7 +25280,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="5" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="5" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>347</v>
       </c>
@@ -25265,7 +25301,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>337</v>
       </c>
@@ -25286,7 +25322,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>411</v>
       </c>
@@ -25309,7 +25345,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>423</v>
       </c>
@@ -25332,7 +25368,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>456</v>
       </c>
@@ -25355,7 +25391,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>500</v>
       </c>
@@ -25378,7 +25414,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="5" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="5" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>535</v>
       </c>
@@ -25407,7 +25443,7 @@
       <c r="L10" s="67"/>
       <c r="M10" s="67"/>
     </row>
-    <row r="11" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>568</v>
       </c>
@@ -25430,7 +25466,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="27" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="27" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A12" s="42" t="s">
         <v>584</v>
       </c>
@@ -25453,7 +25489,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="27" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="27" customFormat="1" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A13" s="42" t="s">
         <v>588</v>
       </c>
@@ -25476,7 +25512,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>702</v>
       </c>
@@ -25499,7 +25535,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="89" t="s">
         <v>337</v>
       </c>
@@ -25522,7 +25558,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="89" t="s">
         <v>711</v>
       </c>
@@ -25545,7 +25581,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="89" t="s">
         <v>682</v>
       </c>
@@ -25562,7 +25598,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A18" s="89" t="s">
         <v>673</v>
       </c>
@@ -25581,7 +25617,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="40.799999999999997" x14ac:dyDescent="0.2">
       <c r="A19" s="89" t="s">
         <v>673</v>
       </c>
@@ -25598,7 +25634,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A20" s="89" t="s">
         <v>763</v>
       </c>
@@ -25615,7 +25651,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A21" s="89" t="s">
         <v>774</v>
       </c>
@@ -25632,7 +25668,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A22" s="89" t="s">
         <v>781</v>
       </c>
@@ -25649,7 +25685,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A23" s="89" t="s">
         <v>784</v>
       </c>
@@ -25666,7 +25702,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A24" s="89" t="s">
         <v>687</v>
       </c>
@@ -25684,7 +25720,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="40.799999999999997" x14ac:dyDescent="0.2">
       <c r="A25" s="89" t="s">
         <v>663</v>
       </c>
@@ -25701,7 +25737,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="40.799999999999997" x14ac:dyDescent="0.2">
       <c r="A26" s="89" t="s">
         <v>692</v>
       </c>
@@ -25718,7 +25754,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A27" s="89" t="s">
         <v>690</v>
       </c>
@@ -25735,7 +25771,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A28" s="89" t="s">
         <v>818</v>
       </c>
@@ -25757,31 +25793,31 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="F4" r:id="rId2"/>
-    <hyperlink ref="F5" r:id="rId3"/>
-    <hyperlink ref="F6" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
-    <hyperlink ref="E7" r:id="rId7"/>
-    <hyperlink ref="F8" r:id="rId8"/>
-    <hyperlink ref="E8" r:id="rId9"/>
-    <hyperlink ref="F9" r:id="rId10"/>
-    <hyperlink ref="E9" r:id="rId11"/>
-    <hyperlink ref="F10" r:id="rId12"/>
-    <hyperlink ref="E10" r:id="rId13"/>
-    <hyperlink ref="F11" r:id="rId14"/>
-    <hyperlink ref="E11" r:id="rId15"/>
-    <hyperlink ref="F12" r:id="rId16"/>
-    <hyperlink ref="E12" r:id="rId17"/>
-    <hyperlink ref="F13" r:id="rId18" location="pdf-link" display="https://journals.lww.com/transplantjournal/fulltext/2009/03270/Donor_Derived_Mesenchymal_Stem_Cells_Suppress.17.aspx - pdf-link"/>
-    <hyperlink ref="E13" r:id="rId19"/>
-    <hyperlink ref="E14" r:id="rId20"/>
-    <hyperlink ref="F14" r:id="rId21"/>
-    <hyperlink ref="F15" r:id="rId22"/>
-    <hyperlink ref="E15" r:id="rId23"/>
-    <hyperlink ref="E16" r:id="rId24"/>
-    <hyperlink ref="F16" r:id="rId25"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="E7" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="F8" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="E8" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="F9" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="E9" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
+    <hyperlink ref="F10" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
+    <hyperlink ref="E10" r:id="rId13" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
+    <hyperlink ref="F11" r:id="rId14" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
+    <hyperlink ref="E11" r:id="rId15" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
+    <hyperlink ref="F12" r:id="rId16" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
+    <hyperlink ref="E12" r:id="rId17" xr:uid="{00000000-0004-0000-0400-000010000000}"/>
+    <hyperlink ref="F13" r:id="rId18" location="pdf-link" display="https://journals.lww.com/transplantjournal/fulltext/2009/03270/Donor_Derived_Mesenchymal_Stem_Cells_Suppress.17.aspx - pdf-link" xr:uid="{00000000-0004-0000-0400-000011000000}"/>
+    <hyperlink ref="E13" r:id="rId19" xr:uid="{00000000-0004-0000-0400-000012000000}"/>
+    <hyperlink ref="E14" r:id="rId20" xr:uid="{00000000-0004-0000-0400-000013000000}"/>
+    <hyperlink ref="F14" r:id="rId21" xr:uid="{00000000-0004-0000-0400-000014000000}"/>
+    <hyperlink ref="F15" r:id="rId22" xr:uid="{00000000-0004-0000-0400-000015000000}"/>
+    <hyperlink ref="E15" r:id="rId23" xr:uid="{00000000-0004-0000-0400-000016000000}"/>
+    <hyperlink ref="E16" r:id="rId24" xr:uid="{00000000-0004-0000-0400-000017000000}"/>
+    <hyperlink ref="F16" r:id="rId25" xr:uid="{00000000-0004-0000-0400-000018000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
@@ -25789,23 +25825,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q62"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="36.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="152" t="s">
         <v>594</v>
       </c>
@@ -25822,7 +25858,7 @@
       <c r="K1" s="154"/>
       <c r="L1" s="154"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
@@ -25833,7 +25869,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -25851,7 +25887,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>26</v>
       </c>
@@ -25887,7 +25923,7 @@
       <c r="P4" s="75"/>
       <c r="Q4" s="75"/>
     </row>
-    <row r="5" spans="1:17" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="42">
         <v>20</v>
       </c>
@@ -25916,7 +25952,7 @@
       <c r="O5" s="151"/>
       <c r="P5" s="151"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>21</v>
       </c>
@@ -25939,7 +25975,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="28">
         <v>17</v>
       </c>
@@ -25968,7 +26004,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>11</v>
       </c>
@@ -25991,7 +26027,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>39</v>
       </c>
@@ -26014,7 +26050,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>33</v>
       </c>
@@ -26037,7 +26073,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>14</v>
       </c>
@@ -26060,7 +26096,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>34</v>
       </c>
@@ -26083,7 +26119,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>27</v>
       </c>
@@ -26106,7 +26142,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>38</v>
       </c>
@@ -26129,7 +26165,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>23</v>
       </c>
@@ -26158,7 +26194,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>13</v>
       </c>
@@ -26181,7 +26217,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>2</v>
       </c>
@@ -26204,7 +26240,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>24</v>
       </c>
@@ -26227,7 +26263,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>8</v>
       </c>
@@ -26250,7 +26286,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>3</v>
       </c>
@@ -26279,7 +26315,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>40</v>
       </c>
@@ -26308,7 +26344,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="32">
         <v>18</v>
       </c>
@@ -26331,7 +26367,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>32</v>
       </c>
@@ -26354,7 +26390,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>1</v>
       </c>
@@ -26377,7 +26413,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>6</v>
       </c>
@@ -26400,7 +26436,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>30</v>
       </c>
@@ -26423,7 +26459,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>9</v>
       </c>
@@ -26446,7 +26482,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>29</v>
       </c>
@@ -26469,7 +26505,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>35</v>
       </c>
@@ -26492,7 +26528,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <v>41</v>
       </c>
@@ -26515,7 +26551,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>10</v>
       </c>
@@ -26538,7 +26574,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>15</v>
       </c>
@@ -26567,7 +26603,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>25</v>
       </c>
@@ -26590,7 +26626,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>4</v>
       </c>
@@ -26616,7 +26652,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>16</v>
       </c>
@@ -26642,7 +26678,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="32">
         <v>19</v>
       </c>
@@ -26665,7 +26701,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>37</v>
       </c>
@@ -26688,7 +26724,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <v>7</v>
       </c>
@@ -26711,7 +26747,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>28</v>
       </c>
@@ -26734,7 +26770,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>5</v>
       </c>
@@ -26757,7 +26793,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>31</v>
       </c>
@@ -26780,7 +26816,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <v>12</v>
       </c>
@@ -26803,7 +26839,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>36</v>
       </c>
@@ -26826,7 +26862,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
         <v>42</v>
       </c>
@@ -26846,7 +26882,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
         <v>22</v>
       </c>
@@ -26875,7 +26911,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -26892,7 +26928,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -26909,7 +26945,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="153" t="s">
         <v>595</v>
       </c>
@@ -26930,7 +26966,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B49" s="42" t="s">
         <v>588</v>
       </c>
@@ -26950,7 +26986,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B50" s="1" t="s">
         <v>456</v>
       </c>
@@ -26970,7 +27006,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B51" s="5" t="s">
         <v>150</v>
       </c>
@@ -26990,7 +27026,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B52" s="7" t="s">
         <v>535</v>
       </c>
@@ -27019,7 +27055,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B53" s="7" t="s">
         <v>337</v>
       </c>
@@ -27039,7 +27075,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B54" s="42" t="s">
         <v>584</v>
       </c>
@@ -27059,7 +27095,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B55" s="1" t="s">
         <v>568</v>
       </c>
@@ -27079,7 +27115,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B56" s="7" t="s">
         <v>347</v>
       </c>
@@ -27099,7 +27135,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B57" s="1" t="s">
         <v>500</v>
       </c>
@@ -27119,7 +27155,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B58" s="1" t="s">
         <v>411</v>
       </c>
@@ -27139,7 +27175,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
         <v>423</v>
       </c>
@@ -27159,7 +27195,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:13" x14ac:dyDescent="0.3">
       <c r="I60" s="77" t="s">
         <v>673</v>
       </c>
@@ -27173,7 +27209,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:13" x14ac:dyDescent="0.3">
       <c r="I61" s="77" t="s">
         <v>692</v>
       </c>
@@ -27187,7 +27223,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:13" x14ac:dyDescent="0.3">
       <c r="I62" s="77" t="s">
         <v>693</v>
       </c>
@@ -27202,7 +27238,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B49:C59">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B49:C59">
     <sortCondition ref="B49:B59"/>
   </sortState>
   <mergeCells count="6">
@@ -27219,18 +27255,18 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A2:B78"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="B42" sqref="B42:B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="64" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -27620,7 +27656,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B76" s="22" t="s">
         <v>421</v>
       </c>
@@ -27639,20 +27675,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="127.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="127.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>261</v>
       </c>
@@ -27663,7 +27699,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>38</v>
       </c>

</xml_diff>